<commit_message>
until lesson1 embedded c
</commit_message>
<xml_diff>
--- a/Quizes.xlsx
+++ b/Quizes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Quizes</t>
   </si>
@@ -24,18 +24,6 @@
     <t>Degree</t>
   </si>
   <si>
-    <t>Quiz1</t>
-  </si>
-  <si>
-    <t>Quiz2</t>
-  </si>
-  <si>
-    <t>Quiz3</t>
-  </si>
-  <si>
-    <t>Quiz4</t>
-  </si>
-  <si>
     <t>30 - 35</t>
   </si>
   <si>
@@ -49,6 +37,30 @@
   </si>
   <si>
     <t>Midterm</t>
+  </si>
+  <si>
+    <t>Quiz1 (C-basics)</t>
+  </si>
+  <si>
+    <t>Quiz4 (Functions)</t>
+  </si>
+  <si>
+    <t>Quiz3 (Conditions &amp; loops)</t>
+  </si>
+  <si>
+    <t>Quiz2 (Arrays &amp; Strings)</t>
+  </si>
+  <si>
+    <t>Quiz8 (Embedded-C)</t>
+  </si>
+  <si>
+    <t>Quiz5 (Struct &amp; Union &amp; Enum)</t>
+  </si>
+  <si>
+    <t>Quiz6 (Preprocecssor directives)</t>
+  </si>
+  <si>
+    <t>Quiz7 (Pointer)</t>
   </si>
 </sst>
 </file>
@@ -387,13 +399,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -403,15 +418,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>60</v>
@@ -419,10 +434,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>36</v>
@@ -430,10 +445,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>40</v>
@@ -441,7 +456,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -452,7 +467,51 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>